<commit_message>
Added MatplotLib page for Doubly Linked List sorting.
</commit_message>
<xml_diff>
--- a/TimeDurationComparisonSortDLL.xlsx
+++ b/TimeDurationComparisonSortDLL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hachidori\PycharmProjects\SortProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFF1671-3017-4D0C-9792-F03756A71D91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D7EB22-FD64-4FE4-ACBD-305254C5CA3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18465" yWindow="405" windowWidth="17265" windowHeight="10800" xr2:uid="{BF59B25C-07BB-4DAF-BB0E-BA360C58BB29}"/>
+    <workbookView xWindow="-17895" yWindow="315" windowWidth="17265" windowHeight="10800" xr2:uid="{BF59B25C-07BB-4DAF-BB0E-BA360C58BB29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -399,7 +399,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,6 +424,9 @@
       <c r="A2" s="1">
         <v>100</v>
       </c>
+      <c r="B2">
+        <v>9.9992752075195291E-4</v>
+      </c>
       <c r="C2">
         <v>3.0000209808349601E-3</v>
       </c>
@@ -431,6 +434,9 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1000</v>
+      </c>
+      <c r="B3">
+        <v>1.9993782043457001E-3</v>
       </c>
       <c r="C3">
         <v>0.23001980781555101</v>

</xml_diff>

<commit_message>
Adding more Timsort pages and also time duration comparisons.
</commit_message>
<xml_diff>
--- a/TimeDurationComparisonSortDLL.xlsx
+++ b/TimeDurationComparisonSortDLL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hachidori\PycharmProjects\SortProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D7EB22-FD64-4FE4-ACBD-305254C5CA3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78580E3-CAB7-4052-BB38-8807CCC98C83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-17895" yWindow="315" windowWidth="17265" windowHeight="10800" xr2:uid="{BF59B25C-07BB-4DAF-BB0E-BA360C58BB29}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,6 +430,9 @@
       <c r="C2">
         <v>3.0000209808349601E-3</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">

</xml_diff>

<commit_message>
Added a 1,000 number sort Timsort page.
</commit_message>
<xml_diff>
--- a/TimeDurationComparisonSortDLL.xlsx
+++ b/TimeDurationComparisonSortDLL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hachidori\PycharmProjects\SortProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78580E3-CAB7-4052-BB38-8807CCC98C83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3A0AA5-89FB-4B8D-BA9A-BC3013E70B9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-17895" yWindow="315" windowWidth="17265" windowHeight="10800" xr2:uid="{BF59B25C-07BB-4DAF-BB0E-BA360C58BB29}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,6 +444,9 @@
       <c r="C3">
         <v>0.23001980781555101</v>
       </c>
+      <c r="D3">
+        <v>6.0009956359863203E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">

</xml_diff>

<commit_message>
Completed the Timsort pages.
</commit_message>
<xml_diff>
--- a/TimeDurationComparisonSortDLL.xlsx
+++ b/TimeDurationComparisonSortDLL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hachidori\PycharmProjects\SortProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3A0AA5-89FB-4B8D-BA9A-BC3013E70B9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714381ED-7DB4-4D06-8D55-68E2BFB0B4B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17895" yWindow="315" windowWidth="17265" windowHeight="10800" xr2:uid="{BF59B25C-07BB-4DAF-BB0E-BA360C58BB29}"/>
+    <workbookView xWindow="-13230" yWindow="315" windowWidth="12600" windowHeight="10800" xr2:uid="{BF59B25C-07BB-4DAF-BB0E-BA360C58BB29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -399,7 +399,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,10 +455,16 @@
       <c r="C4">
         <v>25.132065296173</v>
       </c>
+      <c r="D4">
+        <v>8.8007450103759696E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>100000</v>
+      </c>
+      <c r="D5">
+        <v>1.1700975894927901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Insertion Sort definition on DLL Insertion Sort pages
</commit_message>
<xml_diff>
--- a/TimeDurationComparisonSortDLL.xlsx
+++ b/TimeDurationComparisonSortDLL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hachidori\PycharmProjects\SortProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C32AF97-CB25-4ADF-9480-3097D92AD4C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EAC305-3E74-4F54-8439-9BD454EA2CFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-13230" yWindow="315" windowWidth="12600" windowHeight="10800" xr2:uid="{BF59B25C-07BB-4DAF-BB0E-BA360C58BB29}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Completed the matplotlib page for the DLL time durations.
</commit_message>
<xml_diff>
--- a/TimeDurationComparisonSortDLL.xlsx
+++ b/TimeDurationComparisonSortDLL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hachidori\PycharmProjects\SortProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EAC305-3E74-4F54-8439-9BD454EA2CFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCBC523-827C-4E90-8D6E-52A6CBE8A01E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13230" yWindow="315" windowWidth="12600" windowHeight="10800" xr2:uid="{BF59B25C-07BB-4DAF-BB0E-BA360C58BB29}"/>
+    <workbookView xWindow="4290" yWindow="0" windowWidth="12600" windowHeight="10800" xr2:uid="{BF59B25C-07BB-4DAF-BB0E-BA360C58BB29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,10 +48,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -77,11 +83,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACEC7535-69DB-4A75-B642-360358145068}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,25 +457,48 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>10000</v>
       </c>
+      <c r="B4">
+        <v>3.998756E-3</v>
+      </c>
       <c r="C4">
-        <v>25.132065296173</v>
+        <v>25.132065300000001</v>
       </c>
       <c r="D4">
-        <v>8.8007450103759696E-2</v>
+        <v>8.8007450000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>100000</v>
       </c>
+      <c r="B5">
+        <v>7.997512E-3</v>
+      </c>
+      <c r="C5">
+        <v>3568.7532725999999</v>
+      </c>
       <c r="D5">
-        <v>1.1700975894927901</v>
-      </c>
+        <v>1.170097589</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>